<commit_message>
Updating docs and tests
</commit_message>
<xml_diff>
--- a/documentation/WSPExtensions.xlsx
+++ b/documentation/WSPExtensions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/Work/Roman/Gentium/WSP variant/font-gentium-wspx/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/Work/Roman/Gentium/WSP variant/font-gentium-wspx/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CDA4CB5-C20A-244D-8E1A-256071CEABD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D05A347-0AC7-554E-BC0B-18D91343E3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17380" yWindow="500" windowWidth="40260" windowHeight="41840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Chars" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="1203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="1245">
   <si>
     <t>Char</t>
   </si>
@@ -3641,6 +3640,132 @@
   </si>
   <si>
     <t>₈₀₀₈</t>
+  </si>
+  <si>
+    <t>EEE0</t>
+  </si>
+  <si>
+    <t>EEE1</t>
+  </si>
+  <si>
+    <t>EEE2</t>
+  </si>
+  <si>
+    <t>EEE3</t>
+  </si>
+  <si>
+    <t>EEE4</t>
+  </si>
+  <si>
+    <t>EEE5</t>
+  </si>
+  <si>
+    <t>EEE6</t>
+  </si>
+  <si>
+    <t>EEE7</t>
+  </si>
+  <si>
+    <t>EEE8</t>
+  </si>
+  <si>
+    <t>EEE9</t>
+  </si>
+  <si>
+    <t>EEEA</t>
+  </si>
+  <si>
+    <t>EEEB</t>
+  </si>
+  <si>
+    <t>EEEC</t>
+  </si>
+  <si>
+    <t>EEED</t>
+  </si>
+  <si>
+    <t>EEEE</t>
+  </si>
+  <si>
+    <t>EEEF</t>
+  </si>
+  <si>
+    <t>EEF0</t>
+  </si>
+  <si>
+    <t>EEF1</t>
+  </si>
+  <si>
+    <t>EEF2</t>
+  </si>
+  <si>
+    <t>EEF3</t>
+  </si>
+  <si>
+    <t>EEFF</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
   </si>
 </sst>
 </file>
@@ -3919,8 +4044,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="F337" sqref="F337"/>
+    <sheetView tabSelected="1" topLeftCell="A346" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="E374" sqref="E374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -20706,11 +20831,24 @@
       <c r="Z376" s="2"/>
     </row>
     <row r="377" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A377" s="2"/>
-      <c r="B377" s="2"/>
-      <c r="C377" s="2"/>
-      <c r="D377" s="2"/>
-      <c r="E377" s="2"/>
+      <c r="A377" s="2" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B377" s="2" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C377" s="2" t="str">
+        <f t="shared" ref="C377:C397" si="5">"OH"&amp;B377&amp;"HO"</f>
+        <v>OHHO</v>
+      </c>
+      <c r="D377" s="2" t="str">
+        <f t="shared" ref="D377:D397" si="6">"no"&amp;B377&amp;"on"</f>
+        <v>noon</v>
+      </c>
+      <c r="E377" s="2" t="str">
+        <f t="shared" ref="E377:E397" si="7">"80"&amp;B377&amp;"08"</f>
+        <v>8008</v>
+      </c>
       <c r="F377" s="2"/>
       <c r="G377" s="2"/>
       <c r="H377" s="2"/>
@@ -20734,11 +20872,24 @@
       <c r="Z377" s="2"/>
     </row>
     <row r="378" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A378" s="2"/>
-      <c r="B378" s="2"/>
-      <c r="C378" s="2"/>
-      <c r="D378" s="2"/>
-      <c r="E378" s="2"/>
+      <c r="A378" s="2" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B378" s="2" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C378" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D378" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E378" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F378" s="2"/>
       <c r="G378" s="2"/>
       <c r="H378" s="2"/>
@@ -20762,11 +20913,24 @@
       <c r="Z378" s="2"/>
     </row>
     <row r="379" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A379" s="2"/>
-      <c r="B379" s="2"/>
-      <c r="C379" s="2"/>
-      <c r="D379" s="2"/>
-      <c r="E379" s="2"/>
+      <c r="A379" s="2" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B379" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C379" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D379" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E379" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F379" s="2"/>
       <c r="G379" s="2"/>
       <c r="H379" s="2"/>
@@ -20790,11 +20954,24 @@
       <c r="Z379" s="2"/>
     </row>
     <row r="380" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A380" s="2"/>
-      <c r="B380" s="2"/>
-      <c r="C380" s="2"/>
-      <c r="D380" s="2"/>
-      <c r="E380" s="2"/>
+      <c r="A380" s="2" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B380" s="2" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C380" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D380" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E380" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F380" s="2"/>
       <c r="G380" s="2"/>
       <c r="H380" s="2"/>
@@ -20818,11 +20995,24 @@
       <c r="Z380" s="2"/>
     </row>
     <row r="381" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A381" s="2"/>
-      <c r="B381" s="2"/>
-      <c r="C381" s="2"/>
-      <c r="D381" s="2"/>
-      <c r="E381" s="2"/>
+      <c r="A381" s="2" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B381" s="2" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C381" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D381" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E381" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F381" s="2"/>
       <c r="G381" s="2"/>
       <c r="H381" s="2"/>
@@ -20846,11 +21036,24 @@
       <c r="Z381" s="2"/>
     </row>
     <row r="382" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A382" s="2"/>
-      <c r="B382" s="2"/>
-      <c r="C382" s="2"/>
-      <c r="D382" s="2"/>
-      <c r="E382" s="2"/>
+      <c r="A382" s="2" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B382" s="2" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C382" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D382" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E382" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F382" s="2"/>
       <c r="G382" s="2"/>
       <c r="H382" s="2"/>
@@ -20874,11 +21077,24 @@
       <c r="Z382" s="2"/>
     </row>
     <row r="383" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A383" s="2"/>
-      <c r="B383" s="2"/>
-      <c r="C383" s="2"/>
-      <c r="D383" s="2"/>
-      <c r="E383" s="2"/>
+      <c r="A383" s="2" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B383" s="2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C383" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D383" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E383" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F383" s="2"/>
       <c r="G383" s="2"/>
       <c r="H383" s="2"/>
@@ -20902,11 +21118,24 @@
       <c r="Z383" s="2"/>
     </row>
     <row r="384" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A384" s="2"/>
-      <c r="B384" s="2"/>
-      <c r="C384" s="2"/>
-      <c r="D384" s="2"/>
-      <c r="E384" s="2"/>
+      <c r="A384" s="2" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B384" s="2" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C384" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D384" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E384" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F384" s="2"/>
       <c r="G384" s="2"/>
       <c r="H384" s="2"/>
@@ -20930,11 +21159,24 @@
       <c r="Z384" s="2"/>
     </row>
     <row r="385" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A385" s="2"/>
-      <c r="B385" s="2"/>
-      <c r="C385" s="2"/>
-      <c r="D385" s="2"/>
-      <c r="E385" s="2"/>
+      <c r="A385" s="2" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B385" s="2" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C385" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D385" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E385" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F385" s="2"/>
       <c r="G385" s="2"/>
       <c r="H385" s="2"/>
@@ -20958,11 +21200,24 @@
       <c r="Z385" s="2"/>
     </row>
     <row r="386" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A386" s="2"/>
-      <c r="B386" s="2"/>
-      <c r="C386" s="2"/>
-      <c r="D386" s="2"/>
-      <c r="E386" s="2"/>
+      <c r="A386" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B386" s="2" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C386" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D386" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E386" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F386" s="2"/>
       <c r="G386" s="2"/>
       <c r="H386" s="2"/>
@@ -20986,11 +21241,24 @@
       <c r="Z386" s="2"/>
     </row>
     <row r="387" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A387" s="2"/>
-      <c r="B387" s="2"/>
-      <c r="C387" s="2"/>
-      <c r="D387" s="2"/>
-      <c r="E387" s="2"/>
+      <c r="A387" s="2" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B387" s="2" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C387" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D387" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E387" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F387" s="2"/>
       <c r="G387" s="2"/>
       <c r="H387" s="2"/>
@@ -21014,11 +21282,24 @@
       <c r="Z387" s="2"/>
     </row>
     <row r="388" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A388" s="2"/>
-      <c r="B388" s="2"/>
-      <c r="C388" s="2"/>
-      <c r="D388" s="2"/>
-      <c r="E388" s="2"/>
+      <c r="A388" s="2" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B388" s="2" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C388" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D388" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E388" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F388" s="2"/>
       <c r="G388" s="2"/>
       <c r="H388" s="2"/>
@@ -21042,11 +21323,24 @@
       <c r="Z388" s="2"/>
     </row>
     <row r="389" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A389" s="2"/>
-      <c r="B389" s="2"/>
-      <c r="C389" s="2"/>
-      <c r="D389" s="2"/>
-      <c r="E389" s="2"/>
+      <c r="A389" s="2" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B389" s="2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C389" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D389" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E389" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F389" s="2"/>
       <c r="G389" s="2"/>
       <c r="H389" s="2"/>
@@ -21070,11 +21364,24 @@
       <c r="Z389" s="2"/>
     </row>
     <row r="390" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A390" s="2"/>
-      <c r="B390" s="2"/>
-      <c r="C390" s="2"/>
-      <c r="D390" s="2"/>
-      <c r="E390" s="2"/>
+      <c r="A390" s="2" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B390" s="2" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C390" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D390" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E390" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F390" s="2"/>
       <c r="G390" s="2"/>
       <c r="H390" s="2"/>
@@ -21098,11 +21405,24 @@
       <c r="Z390" s="2"/>
     </row>
     <row r="391" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A391" s="2"/>
-      <c r="B391" s="2"/>
-      <c r="C391" s="2"/>
-      <c r="D391" s="2"/>
-      <c r="E391" s="2"/>
+      <c r="A391" s="2" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B391" s="2" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C391" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D391" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E391" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F391" s="2"/>
       <c r="G391" s="2"/>
       <c r="H391" s="2"/>
@@ -21126,11 +21446,24 @@
       <c r="Z391" s="2"/>
     </row>
     <row r="392" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A392" s="2"/>
-      <c r="B392" s="2"/>
-      <c r="C392" s="2"/>
-      <c r="D392" s="2"/>
-      <c r="E392" s="2"/>
+      <c r="A392" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B392" s="2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C392" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D392" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E392" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F392" s="2"/>
       <c r="G392" s="2"/>
       <c r="H392" s="2"/>
@@ -21154,11 +21487,24 @@
       <c r="Z392" s="2"/>
     </row>
     <row r="393" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A393" s="2"/>
-      <c r="B393" s="2"/>
-      <c r="C393" s="2"/>
-      <c r="D393" s="2"/>
-      <c r="E393" s="2"/>
+      <c r="A393" s="2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B393" s="2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C393" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D393" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E393" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F393" s="2"/>
       <c r="G393" s="2"/>
       <c r="H393" s="2"/>
@@ -21182,11 +21528,24 @@
       <c r="Z393" s="2"/>
     </row>
     <row r="394" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A394" s="2"/>
-      <c r="B394" s="2"/>
-      <c r="C394" s="2"/>
-      <c r="D394" s="2"/>
-      <c r="E394" s="2"/>
+      <c r="A394" s="2" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B394" s="2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C394" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D394" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E394" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F394" s="2"/>
       <c r="G394" s="2"/>
       <c r="H394" s="2"/>
@@ -21210,11 +21569,24 @@
       <c r="Z394" s="2"/>
     </row>
     <row r="395" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A395" s="2"/>
-      <c r="B395" s="2"/>
-      <c r="C395" s="2"/>
-      <c r="D395" s="2"/>
-      <c r="E395" s="2"/>
+      <c r="A395" s="2" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B395" s="2" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C395" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D395" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E395" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F395" s="2"/>
       <c r="G395" s="2"/>
       <c r="H395" s="2"/>
@@ -21238,11 +21610,24 @@
       <c r="Z395" s="2"/>
     </row>
     <row r="396" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A396" s="2"/>
-      <c r="B396" s="2"/>
-      <c r="C396" s="2"/>
-      <c r="D396" s="2"/>
-      <c r="E396" s="2"/>
+      <c r="A396" s="2" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B396" s="2" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C396" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D396" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E396" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F396" s="2"/>
       <c r="G396" s="2"/>
       <c r="H396" s="2"/>
@@ -21266,11 +21651,24 @@
       <c r="Z396" s="2"/>
     </row>
     <row r="397" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A397" s="2"/>
-      <c r="B397" s="2"/>
-      <c r="C397" s="2"/>
-      <c r="D397" s="2"/>
-      <c r="E397" s="2"/>
+      <c r="A397" s="2" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B397" s="2" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C397" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>OHHO</v>
+      </c>
+      <c r="D397" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>noon</v>
+      </c>
+      <c r="E397" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>8008</v>
+      </c>
       <c r="F397" s="2"/>
       <c r="G397" s="2"/>
       <c r="H397" s="2"/>

</xml_diff>